<commit_message>
Flask & SQL - relatie WERKT
</commit_message>
<xml_diff>
--- a/db-structure.xlsx
+++ b/db-structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hanzenl-my.sharepoint.com/personal/a_joseph_st_hanze_nl/Documents/Webtechnologie/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F45B47F-CA83-E247-B9C2-D94498FDBEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{9F45B47F-CA83-E247-B9C2-D94498FDBEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4FD4B65-CB91-3241-A7DE-E4E4C32BCC5C}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="4760" windowWidth="28040" windowHeight="16180" xr2:uid="{84A006C3-8CC1-4343-ADC4-9AEA74A6F9D5}"/>
+    <workbookView xWindow="28800" yWindow="20800" windowWidth="21000" windowHeight="16100" xr2:uid="{84A006C3-8CC1-4343-ADC4-9AEA74A6F9D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Huisjes</t>
   </si>
@@ -44,9 +44,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t xml:space="preserve">type </t>
   </si>
   <si>
@@ -57,6 +54,21 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>naam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reservering </t>
+  </si>
+  <si>
+    <t>datum</t>
+  </si>
+  <si>
+    <t>reservering</t>
+  </si>
+  <si>
+    <t>huisje</t>
   </si>
 </sst>
 </file>
@@ -100,9 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,6 +131,379 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C2638BC-8A17-CC4B-9182-C153F6958BA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2743200" y="1460500"/>
+          <a:ext cx="0" cy="825500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19CCA5D3-6C38-D244-A091-AFEAAA28BD90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="1028700" y="457200"/>
+          <a:ext cx="787400" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Elbow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B342158-0D14-06DE-30EE-051A3274CEAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="812800" y="723900"/>
+          <a:ext cx="2717800" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 111682"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{998040FC-BF15-F787-AB8D-F0864BFC8E0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3530600" y="622300"/>
+          <a:ext cx="0" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Straight Arrow Connector 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB8E03F-3A08-4C36-7852-7817AF3620F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1244600" y="1384300"/>
+          <a:ext cx="0" cy="444500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Connector 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD9F06B6-3E89-F0C2-285C-99EC7279DFAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="1816100"/>
+          <a:ext cx="3289300" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Connector 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B36F5520-0E6B-704B-A0AD-E0F549DA4733}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4432300" y="1828800"/>
+          <a:ext cx="12700" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,47 +803,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF913E9-BBD9-9B4E-959D-363EF717B1DA}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
+      <c r="F12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>